<commit_message>
update function added for db
</commit_message>
<xml_diff>
--- a/source_tfvc_permissions.xlsx
+++ b/source_tfvc_permissions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="26">
   <si>
     <t>Permissions</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>CatCore Build Service (DefaultCollection)</t>
+  </si>
+  <si>
+    <t>CatCore Team</t>
   </si>
 </sst>
 </file>
@@ -429,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -437,16 +440,17 @@
   <cols>
     <col min="1" max="1" width="37.7109375" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="24.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
     <col min="6" max="6" width="35.7109375" customWidth="1"/>
     <col min="7" max="7" width="43.7109375" customWidth="1"/>
-    <col min="8" max="8" width="37.7109375" customWidth="1"/>
+    <col min="8" max="8" width="43.7109375" customWidth="1"/>
     <col min="9" max="9" width="43.7109375" customWidth="1"/>
+    <col min="10" max="10" width="43.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,8 +478,11 @@
       <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -486,7 +493,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -503,19 +510,22 @@
       <c r="I2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -530,10 +540,13 @@
         <v>21</v>
       </c>
       <c r="I3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -544,7 +557,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
@@ -559,21 +572,24 @@
         <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
@@ -588,21 +604,24 @@
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>21</v>
+      </c>
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
         <v>3</v>
@@ -617,10 +636,13 @@
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -631,7 +653,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
         <v>3</v>
@@ -646,10 +668,13 @@
         <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>21</v>
+      </c>
+      <c r="J7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -660,7 +685,7 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
         <v>3</v>
@@ -677,19 +702,22 @@
       <c r="I8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
         <v>3</v>
@@ -704,21 +732,24 @@
         <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>21</v>
+      </c>
+      <c r="J9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
         <v>3</v>
@@ -733,24 +764,27 @@
         <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>21</v>
+      </c>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
         <v>21</v>
@@ -762,10 +796,13 @@
         <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>21</v>
+      </c>
+      <c r="J11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -776,7 +813,7 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E12" t="s">
         <v>3</v>
@@ -793,8 +830,11 @@
       <c r="I12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -805,7 +845,7 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
         <v>3</v>
@@ -822,8 +862,11 @@
       <c r="I13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -834,7 +877,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
@@ -849,6 +892,9 @@
         <v>21</v>
       </c>
       <c r="I14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>